<commit_message>
update fix some bug with categoryList -> change it to dynamic, update upload to cloudinary with chunk size
</commit_message>
<xml_diff>
--- a/TestCase/testCaseNodeJS.xlsx
+++ b/TestCase/testCaseNodeJS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="247">
   <si>
     <t>Test Requirement List</t>
   </si>
@@ -2712,6 +2712,9 @@
   <si>
     <t>Phone: Không thành công
 Email:thành công</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
   <si>
     <t>TC_UM_004</t>
@@ -15812,6 +15815,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <charset val="0"/>
+      </rPr>
       <t>1. ch</t>
     </r>
     <r>
@@ -15984,6 +15992,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <charset val="0"/>
+      </rPr>
       <t>1. ch</t>
     </r>
     <r>
@@ -16075,6 +16088,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <charset val="0"/>
+      </rPr>
       <t>Em có th</t>
     </r>
     <r>
@@ -16174,6 +16192,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <charset val="0"/>
+      </rPr>
       <t>C</t>
     </r>
     <r>
@@ -16211,6 +16234,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <charset val="0"/>
+      </rPr>
       <t>c</t>
     </r>
     <r>
@@ -16251,6 +16279,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <charset val="0"/>
+      </rPr>
       <t>1. ch</t>
     </r>
     <r>
@@ -16355,6 +16388,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <charset val="0"/>
+      </rPr>
       <t>C</t>
     </r>
     <r>
@@ -16456,6 +16494,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <charset val="0"/>
+      </rPr>
       <t>D</t>
     </r>
     <r>
@@ -16670,7 +16713,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -16722,13 +16765,6 @@
     <font>
       <strike/>
       <sz val="10"/>
-      <name val="Trebuchet MS"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Trebuchet MS"/>
       <charset val="0"/>
     </font>
@@ -17259,13 +17295,16 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -17274,122 +17313,119 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -17484,9 +17520,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -18045,8 +18078,8 @@
   <sheetPr/>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="B65" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -18410,8 +18443,8 @@
       <c r="F16" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="29" t="s">
-        <v>18</v>
+      <c r="G16" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="24" t="s">
@@ -18422,19 +18455,19 @@
     <row r="17" ht="72" spans="1:10">
       <c r="A17" s="19"/>
       <c r="B17" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G17" s="28" t="s">
         <v>18</v>
@@ -18448,19 +18481,19 @@
     <row r="18" ht="43.2" spans="1:10">
       <c r="A18" s="19"/>
       <c r="B18" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G18" s="28" t="s">
         <v>18</v>
@@ -18474,19 +18507,19 @@
     <row r="19" ht="57.6" spans="1:10">
       <c r="A19" s="19"/>
       <c r="B19" s="26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>18</v>
@@ -18500,103 +18533,103 @@
     <row r="20" ht="57.6" spans="1:10">
       <c r="A20" s="19"/>
       <c r="B20" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>18</v>
+        <v>73</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" ht="57.6" spans="1:10">
       <c r="A21" s="19"/>
       <c r="B21" s="26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>18</v>
+        <v>73</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" ht="57.6" spans="1:10">
       <c r="A22" s="19"/>
       <c r="B22" s="26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>18</v>
+        <v>79</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H22" s="26"/>
       <c r="I22" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" ht="86.4" spans="1:10">
       <c r="A23" s="19"/>
       <c r="B23" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G23" s="28" t="s">
         <v>18</v>
@@ -18610,19 +18643,19 @@
     <row r="24" ht="57.6" spans="1:10">
       <c r="A24" s="19"/>
       <c r="B24" s="26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G24" s="28" t="s">
         <v>18</v>
@@ -18632,25 +18665,25 @@
         <v>19</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" ht="43.2" spans="1:10">
       <c r="A25" s="19"/>
       <c r="B25" s="26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G25" s="28" t="s">
         <v>18</v>
@@ -18660,7 +18693,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -18677,7 +18710,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="14"/>
@@ -18692,47 +18725,47 @@
     <row r="28" ht="187.2" spans="1:10">
       <c r="A28" s="19"/>
       <c r="B28" s="20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="G28" s="31" t="s">
-        <v>18</v>
+        <v>98</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>58</v>
       </c>
       <c r="H28" s="26"/>
       <c r="I28" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" ht="43.2" spans="1:10">
       <c r="A29" s="19"/>
       <c r="B29" s="26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>35</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G29" s="28" t="s">
         <v>18</v>
@@ -18746,19 +18779,19 @@
     <row r="30" ht="43.2" spans="1:10">
       <c r="A30" s="19"/>
       <c r="B30" s="26" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G30" s="28" t="s">
         <v>18</v>
@@ -18772,19 +18805,19 @@
     <row r="31" ht="57.6" spans="1:10">
       <c r="A31" s="19"/>
       <c r="B31" s="26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G31" s="28" t="s">
         <v>18</v>
@@ -18798,62 +18831,62 @@
     <row r="32" ht="57.6" spans="1:10">
       <c r="A32" s="19"/>
       <c r="B32" s="26" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>53</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="G32" s="29" t="s">
-        <v>18</v>
+        <v>113</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H32" s="26"/>
       <c r="I32" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" ht="57.6" spans="1:10">
       <c r="A33" s="19"/>
       <c r="B33" s="26" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D33" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>18</v>
+        <v>117</v>
+      </c>
+      <c r="G33" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J33" s="24" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="14"/>
@@ -18868,22 +18901,22 @@
     <row r="35" ht="43.2" spans="1:10">
       <c r="A35" s="19"/>
       <c r="B35" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D35" s="30" t="s">
         <v>35</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="G35" s="31" t="s">
-        <v>18</v>
+        <v>123</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>58</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="24" t="s">
@@ -18894,19 +18927,19 @@
     <row r="36" ht="43.2" spans="1:10">
       <c r="A36" s="19"/>
       <c r="B36" s="26" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G36" s="28" t="s">
         <v>18</v>
@@ -18920,19 +18953,19 @@
     <row r="37" ht="43.2" spans="1:10">
       <c r="A37" s="19"/>
       <c r="B37" s="26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G37" s="28" t="s">
         <v>18</v>
@@ -18946,19 +18979,19 @@
     <row r="38" ht="57.6" spans="1:10">
       <c r="A38" s="19"/>
       <c r="B38" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D38" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G38" s="28" t="s">
         <v>18</v>
@@ -18972,34 +19005,34 @@
     <row r="39" ht="57.6" spans="1:10">
       <c r="A39" s="19"/>
       <c r="B39" s="26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D39" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>18</v>
+        <v>136</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J39" s="26" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="14"/>
@@ -19014,19 +19047,19 @@
     <row r="41" ht="43.2" spans="1:10">
       <c r="A41" s="19"/>
       <c r="B41" s="20" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G41" s="25" t="s">
         <v>18</v>
@@ -19040,19 +19073,19 @@
     <row r="42" ht="43.2" spans="1:10">
       <c r="A42" s="19"/>
       <c r="B42" s="26" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G42" s="28" t="s">
         <v>18</v>
@@ -19066,19 +19099,19 @@
     <row r="43" ht="43.2" spans="1:10">
       <c r="A43" s="19"/>
       <c r="B43" s="26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D43" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G43" s="28" t="s">
         <v>18</v>
@@ -19092,19 +19125,19 @@
     <row r="44" ht="43.2" spans="1:10">
       <c r="A44" s="19"/>
       <c r="B44" s="26" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D44" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G44" s="28" t="s">
         <v>18</v>
@@ -19118,19 +19151,19 @@
     <row r="45" ht="57.6" spans="1:10">
       <c r="A45" s="19"/>
       <c r="B45" s="26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G45" s="28" t="s">
         <v>18</v>
@@ -19144,19 +19177,19 @@
     <row r="46" ht="43.2" spans="1:10">
       <c r="A46" s="19"/>
       <c r="B46" s="26" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D46" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G46" s="28" t="s">
         <v>18</v>
@@ -19166,25 +19199,25 @@
         <v>19</v>
       </c>
       <c r="J46" s="24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" ht="28.8" spans="1:10">
       <c r="A47" s="19"/>
       <c r="B47" s="26" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D47" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G47" s="28" t="s">
         <v>18</v>
@@ -19198,19 +19231,19 @@
     <row r="48" ht="43.2" spans="1:10">
       <c r="A48" s="19"/>
       <c r="B48" s="26" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D48" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G48" s="28" t="s">
         <v>18</v>
@@ -19219,54 +19252,54 @@
       <c r="I48" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J48" s="32" t="s">
-        <v>169</v>
+      <c r="J48" s="31" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="49" ht="57.6" spans="1:10">
       <c r="A49" s="19"/>
       <c r="B49" s="26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D49" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="G49" s="29" t="s">
-        <v>18</v>
+        <v>79</v>
+      </c>
+      <c r="G49" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H49" s="26"/>
       <c r="I49" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J49" s="24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" ht="86.4" spans="1:10">
       <c r="A50" s="19"/>
       <c r="B50" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G50" s="28" t="s">
         <v>18</v>
@@ -19280,19 +19313,19 @@
     <row r="51" ht="57.6" spans="1:10">
       <c r="A51" s="19"/>
       <c r="B51" s="26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D51" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G51" s="28" t="s">
         <v>18</v>
@@ -19302,25 +19335,25 @@
         <v>19</v>
       </c>
       <c r="J51" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" ht="43.2" spans="1:10">
       <c r="A52" s="19"/>
       <c r="B52" s="26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D52" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G52" s="28" t="s">
         <v>18</v>
@@ -19330,12 +19363,12 @@
         <v>19</v>
       </c>
       <c r="J52" s="24" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="14"/>
@@ -19350,19 +19383,19 @@
     <row r="54" ht="115.2" spans="1:10">
       <c r="A54" s="19"/>
       <c r="B54" s="20" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G54" s="25" t="s">
         <v>18</v>
@@ -19372,25 +19405,25 @@
         <v>19</v>
       </c>
       <c r="J54" s="24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" ht="57.6" spans="1:10">
       <c r="A55" s="19"/>
       <c r="B55" s="26" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G55" s="28" t="s">
         <v>18</v>
@@ -19400,25 +19433,25 @@
         <v>19</v>
       </c>
       <c r="J55" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="56" ht="86.4" spans="1:10">
       <c r="A56" s="19"/>
       <c r="B56" s="26" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G56" s="28" t="s">
         <v>18</v>
@@ -19428,25 +19461,25 @@
         <v>19</v>
       </c>
       <c r="J56" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" ht="57.6" spans="1:10">
       <c r="A57" s="19"/>
       <c r="B57" s="26" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G57" s="28" t="s">
         <v>18</v>
@@ -19460,19 +19493,19 @@
     <row r="58" ht="57.6" spans="1:10">
       <c r="A58" s="19"/>
       <c r="B58" s="26" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G58" s="28" t="s">
         <v>18</v>
@@ -19482,53 +19515,53 @@
         <v>19</v>
       </c>
       <c r="J58" s="26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" ht="57.6" spans="1:10">
       <c r="A59" s="19"/>
       <c r="B59" s="26" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="G59" s="29" t="s">
-        <v>18</v>
+        <v>201</v>
+      </c>
+      <c r="G59" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H59" s="26"/>
       <c r="I59" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J59" s="24" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" ht="57.6" spans="1:10">
       <c r="A60" s="19"/>
       <c r="B60" s="26" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G60" s="28" t="s">
         <v>18</v>
@@ -19538,53 +19571,53 @@
         <v>19</v>
       </c>
       <c r="J60" s="26" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" ht="72" spans="1:10">
       <c r="A61" s="19"/>
       <c r="B61" s="26" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>210</v>
-      </c>
-      <c r="G61" s="29" t="s">
-        <v>18</v>
+        <v>211</v>
+      </c>
+      <c r="G61" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H61" s="26"/>
       <c r="I61" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J61" s="32" t="s">
-        <v>211</v>
+      <c r="J61" s="31" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="62" ht="72" spans="1:10">
       <c r="A62" s="19"/>
       <c r="B62" s="26" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G62" s="28" t="s">
         <v>18</v>
@@ -19594,53 +19627,53 @@
         <v>19</v>
       </c>
       <c r="J62" s="24" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" ht="86.4" spans="1:10">
       <c r="A63" s="19"/>
       <c r="B63" s="26" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="G63" s="29" t="s">
-        <v>18</v>
+        <v>222</v>
+      </c>
+      <c r="G63" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H63" s="26"/>
       <c r="I63" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J63" s="24" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" ht="72" spans="1:10">
       <c r="A64" s="19"/>
       <c r="B64" s="26" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G64" s="28" t="s">
         <v>18</v>
@@ -19649,26 +19682,26 @@
       <c r="I64" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J64" s="32" t="s">
-        <v>227</v>
+      <c r="J64" s="31" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="65" ht="57.6" spans="1:10">
       <c r="A65" s="19"/>
       <c r="B65" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C65" s="27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G65" s="28" t="s">
         <v>18</v>
@@ -19681,7 +19714,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B66" s="13"/>
       <c r="C66" s="14"/>
@@ -19696,19 +19729,19 @@
     <row r="67" ht="57.6" spans="1:10">
       <c r="A67" s="19"/>
       <c r="B67" s="20" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G67" s="25" t="s">
         <v>18</v>
@@ -19718,25 +19751,25 @@
         <v>19</v>
       </c>
       <c r="J67" s="24" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="68" ht="57.6" spans="1:10">
       <c r="A68" s="19"/>
       <c r="B68" s="26" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D68" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E68" s="23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G68" s="28" t="s">
         <v>18</v>
@@ -19750,19 +19783,19 @@
     <row r="69" ht="57.6" spans="1:10">
       <c r="A69" s="19"/>
       <c r="B69" s="26" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D69" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E69" s="23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G69" s="28" t="s">
         <v>18</v>
@@ -19776,29 +19809,29 @@
     <row r="70" ht="57.6" spans="1:10">
       <c r="A70" s="19"/>
       <c r="B70" s="26" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C70" s="27" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D70" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="G70" s="29" t="s">
-        <v>18</v>
+        <v>245</v>
+      </c>
+      <c r="G70" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="H70" s="26"/>
       <c r="I70" s="24" t="s">
         <v>19</v>
       </c>
       <c r="J70" s="26" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -19847,7 +19880,7 @@
       <c r="G74" s="29"/>
       <c r="H74" s="26"/>
       <c r="I74" s="24"/>
-      <c r="J74" s="32"/>
+      <c r="J74" s="31"/>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="19"/>
@@ -19883,7 +19916,7 @@
       <c r="G77" s="28"/>
       <c r="H77" s="26"/>
       <c r="I77" s="24"/>
-      <c r="J77" s="32"/>
+      <c r="J77" s="31"/>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="19"/>

</xml_diff>